<commit_message>
separate pre and data
</commit_message>
<xml_diff>
--- a/data/raw/varnames.xlsx
+++ b/data/raw/varnames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickgirdwood/r/traildata/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B670D566-AF07-9E40-BF35-08A2A7978C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA2E643-FB92-9746-8118-B534B3DE5BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35060" yWindow="40" windowWidth="28800" windowHeight="17500" xr2:uid="{F7BF8602-2FA3-994F-9E79-F4296B4BA099}"/>
+    <workbookView xWindow="35060" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{F7BF8602-2FA3-994F-9E79-F4296B4BA099}"/>
   </bookViews>
   <sheets>
     <sheet name="koos" sheetId="1" r:id="rId1"/>
@@ -1009,9 +1009,6 @@
     <t>training_stretch</t>
   </si>
   <si>
-    <t>training_strwtch_freq</t>
-  </si>
-  <si>
     <t>covid_runningvolume</t>
   </si>
   <si>
@@ -2616,6 +2613,9 @@
   </si>
   <si>
     <t>koos_q_total</t>
+  </si>
+  <si>
+    <t>training_stretch_freq</t>
   </si>
 </sst>
 </file>
@@ -2664,12 +2664,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2987,7 +2986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5319468-0651-CB48-84DD-4DB55BDF580F}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3009,7 +3008,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3017,7 +3016,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3025,7 +3024,7 @@
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3033,7 +3032,7 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3041,7 +3040,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3049,7 +3048,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3057,7 +3056,7 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3065,7 +3064,7 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3073,7 +3072,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3081,7 +3080,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3089,7 +3088,7 @@
         <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3097,7 +3096,7 @@
         <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3105,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="68" x14ac:dyDescent="0.2">
@@ -3113,7 +3112,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3121,7 +3120,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3129,7 +3128,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3137,7 +3136,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3145,7 +3144,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3153,7 +3152,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3161,7 +3160,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3169,7 +3168,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3177,7 +3176,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3185,7 +3184,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3193,7 +3192,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3201,7 +3200,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3209,7 +3208,7 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3217,7 +3216,7 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -3225,7 +3224,7 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3233,7 +3232,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3241,7 +3240,7 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3249,7 +3248,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3257,7 +3256,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3265,7 +3264,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3273,7 +3272,7 @@
         <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="68" x14ac:dyDescent="0.2">
@@ -3281,15 +3280,15 @@
         <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B37" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -3297,7 +3296,7 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -3305,7 +3304,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -3313,7 +3312,7 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3321,7 +3320,7 @@
         <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -3329,15 +3328,15 @@
         <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -3345,7 +3344,7 @@
         <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -3353,7 +3352,7 @@
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -3361,7 +3360,7 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -3369,7 +3368,7 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3377,7 +3376,7 @@
         <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -3385,7 +3384,7 @@
         <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -3393,7 +3392,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -3401,7 +3400,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -3409,15 +3408,15 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -3425,7 +3424,7 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -3433,7 +3432,7 @@
         <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -3441,7 +3440,7 @@
         <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -3449,7 +3448,7 @@
         <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -3457,7 +3456,7 @@
         <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -3465,7 +3464,7 @@
         <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -3473,7 +3472,7 @@
         <v>45</v>
       </c>
       <c r="B60" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -3513,55 +3512,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B8" t="s">
         <v>289</v>
@@ -3569,7 +3568,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B9" t="s">
         <v>290</v>
@@ -3577,1138 +3576,1138 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B10" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>450</v>
       </c>
-      <c r="B10" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>451</v>
-      </c>
       <c r="B11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B13" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B14" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B15" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B16" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B18" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B21" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B24" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B25" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B26" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B29" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B35" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B36" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B39" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B40" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B41" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B42" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B43" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B44" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B45" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B46" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B47" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B48" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B49" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B50" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B51" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B52" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B53" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B54" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B55" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B56" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B57" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B58" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B59" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B60" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B61" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B62" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B63" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B64" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B65" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B66" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B67" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B68" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B69" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B70" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B71" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B72" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B73" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B74" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B75" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B76" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B77" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B78" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B79" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B80" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B81" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B82" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B83" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B84" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B85" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B86" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B87" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B88" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B89" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B90" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B91" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B92" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B93" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B94" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B95" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B96" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B97" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B98" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B99" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B100" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B101" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B102" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B103" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B104" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B105" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B106" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B107" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B108" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B109" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B110" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B111" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B112" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B113" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B114" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B115" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B116" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B117" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B118" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B119" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B120" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B121" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B122" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B123" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B124" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B125" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B127" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B128" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B129" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B130" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B131" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B132" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B133" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B134" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B135" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B136" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B137" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B138" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B139" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B140" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B141" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B142" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B143" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B144" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B145" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B146" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B147" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B148" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B149" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B150" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B151" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -4736,210 +4735,210 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B5" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B6" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B8" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B11" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B13" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B14" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B16" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B18" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B19" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B21" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B22" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B23" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B24" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>763</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>789</v>
+        <v>762</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B26" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B27" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>
@@ -5374,170 +5373,170 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>156</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>160</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>164</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5710,8 +5709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271D06C8-E610-FE49-929B-38258FE943CA}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5726,10 +5725,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5769,7 +5768,7 @@
         <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -5777,7 +5776,7 @@
         <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5809,7 +5808,7 @@
         <v>223</v>
       </c>
       <c r="B12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5865,7 +5864,7 @@
         <v>230</v>
       </c>
       <c r="B19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -5897,7 +5896,7 @@
         <v>234</v>
       </c>
       <c r="B23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -6001,7 +6000,7 @@
         <v>247</v>
       </c>
       <c r="B36" t="s">
-        <v>317</v>
+        <v>852</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -6009,7 +6008,7 @@
         <v>248</v>
       </c>
       <c r="B37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -6017,7 +6016,7 @@
         <v>249</v>
       </c>
       <c r="B38" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -6025,7 +6024,7 @@
         <v>250</v>
       </c>
       <c r="B39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -6033,7 +6032,7 @@
         <v>251</v>
       </c>
       <c r="B40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -6041,7 +6040,7 @@
         <v>252</v>
       </c>
       <c r="B41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -6049,7 +6048,7 @@
         <v>253</v>
       </c>
       <c r="B42" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -6057,7 +6056,7 @@
         <v>254</v>
       </c>
       <c r="B43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -6065,7 +6064,7 @@
         <v>255</v>
       </c>
       <c r="B44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -6073,7 +6072,7 @@
         <v>256</v>
       </c>
       <c r="B45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -6081,7 +6080,7 @@
         <v>257</v>
       </c>
       <c r="B46" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -6089,7 +6088,7 @@
         <v>258</v>
       </c>
       <c r="B47" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -6097,7 +6096,7 @@
         <v>259</v>
       </c>
       <c r="B48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -6105,7 +6104,7 @@
         <v>260</v>
       </c>
       <c r="B49" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -6113,7 +6112,7 @@
         <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -6121,7 +6120,7 @@
         <v>262</v>
       </c>
       <c r="B51" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -6129,7 +6128,7 @@
         <v>263</v>
       </c>
       <c r="B52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -6137,7 +6136,7 @@
         <v>264</v>
       </c>
       <c r="B53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -6145,7 +6144,7 @@
         <v>265</v>
       </c>
       <c r="B54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -6153,7 +6152,7 @@
         <v>266</v>
       </c>
       <c r="B55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -6161,7 +6160,7 @@
         <v>267</v>
       </c>
       <c r="B56" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -6169,7 +6168,7 @@
         <v>268</v>
       </c>
       <c r="B57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -6177,7 +6176,7 @@
         <v>269</v>
       </c>
       <c r="B58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -6185,7 +6184,7 @@
         <v>270</v>
       </c>
       <c r="B59" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -6193,7 +6192,7 @@
         <v>271</v>
       </c>
       <c r="B60" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -6201,7 +6200,7 @@
         <v>272</v>
       </c>
       <c r="B61" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -6209,7 +6208,7 @@
         <v>273</v>
       </c>
       <c r="B62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -6217,7 +6216,7 @@
         <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -6225,7 +6224,7 @@
         <v>275</v>
       </c>
       <c r="B64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -6233,7 +6232,7 @@
         <v>276</v>
       </c>
       <c r="B65" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -6241,7 +6240,7 @@
         <v>277</v>
       </c>
       <c r="B66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -6249,7 +6248,7 @@
         <v>278</v>
       </c>
       <c r="B67" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -6257,7 +6256,7 @@
         <v>279</v>
       </c>
       <c r="B68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -6273,7 +6272,7 @@
         <v>281</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -6281,7 +6280,7 @@
         <v>282</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -6297,7 +6296,7 @@
         <v>284</v>
       </c>
       <c r="B73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -6305,7 +6304,7 @@
         <v>285</v>
       </c>
       <c r="B74" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -6313,7 +6312,7 @@
         <v>286</v>
       </c>
       <c r="B75" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -6321,7 +6320,7 @@
         <v>287</v>
       </c>
       <c r="B76" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -6329,7 +6328,7 @@
         <v>288</v>
       </c>
       <c r="B77" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
   </sheetData>
@@ -6358,42 +6357,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -6401,7 +6400,7 @@
         <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -6409,12 +6408,12 @@
         <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B9" t="s">
         <v>292</v>
@@ -6422,10 +6421,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -6433,7 +6432,7 @@
         <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -6441,7 +6440,7 @@
         <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -6449,7 +6448,7 @@
         <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -6457,7 +6456,7 @@
         <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -6465,7 +6464,7 @@
         <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -6473,263 +6472,263 @@
         <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B26" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B36" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B38" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B40" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B45" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B46" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>